<commit_message>
updated Item Register with Excel file
</commit_message>
<xml_diff>
--- a/Data Files/items.xlsx
+++ b/Data Files/items.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -34,20 +34,20 @@
     <t>SMALL PACKS</t>
   </si>
   <si>
-    <t>PEN</t>
-  </si>
-  <si>
-    <t>PENCIL</t>
-  </si>
-  <si>
-    <t>MARKER</t>
+    <t>BISCUT</t>
+  </si>
+  <si>
+    <t>TOFEE</t>
+  </si>
+  <si>
+    <t>CAKE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,7 +167,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -202,7 +201,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -378,21 +376,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -406,12 +404,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1001</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -420,7 +418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -434,12 +432,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>1003</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>

</xml_diff>